<commit_message>
bug fixes for import drink and food
</commit_message>
<xml_diff>
--- a/public/XSWorld_sample_data.xlsx
+++ b/public/XSWorld_sample_data.xlsx
@@ -4,28 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="16275" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="16275" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Items" sheetId="1" r:id="rId1"/>
+    <sheet name="Variations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>product_type</t>
-  </si>
-  <si>
-    <t>category_id</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -68,15 +62,6 @@
     <t>Melbourne</t>
   </si>
   <si>
-    <t>is_available</t>
-  </si>
-  <si>
-    <t>is_featured</t>
-  </si>
-  <si>
-    <t>is_variable</t>
-  </si>
-  <si>
     <t>variation_name</t>
   </si>
   <si>
@@ -95,10 +80,29 @@
     <t>Product No</t>
   </si>
   <si>
-    <t>test Food 1</t>
-  </si>
-  <si>
-    <t>Test Food 2</t>
+    <t>New Drink</t>
+  </si>
+  <si>
+    <t>New Drink 2</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Spirits</t>
+  </si>
+  <si>
+    <t>is_available
+(Item is available or not)</t>
+  </si>
+  <si>
+    <t>is_featured
+(is feature for feature list)</t>
+  </si>
+  <si>
+    <t>is_variable
+(is variable for variations
+You can add variations data in Variation Sheet)</t>
   </si>
 </sst>
 </file>
@@ -140,9 +144,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,149 +444,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12" ht="165">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>19</v>
+      <c r="G2">
+        <v>1996</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>80</v>
-      </c>
-      <c r="E2">
-        <v>120</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>1996</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>110</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>1997</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3">
         <v>0</v>
       </c>
-      <c r="D3" s="1">
-        <v>80</v>
-      </c>
-      <c r="E3">
-        <v>110</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3">
-        <v>1997</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
         <v>0</v>
       </c>
     </row>
@@ -593,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -606,13 +605,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -620,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -631,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -642,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>15</v>

</xml_diff>

<commit_message>
bug fixes for import and change text restaurant intoxication to cancelled
</commit_message>
<xml_diff>
--- a/public/XSWorld_sample_data.xlsx
+++ b/public/XSWorld_sample_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="16275" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="16275" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -47,9 +47,6 @@
     <t>spirit</t>
   </si>
   <si>
-    <t>hello description</t>
-  </si>
-  <si>
     <t>test2</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Wine</t>
   </si>
   <si>
-    <t>Melbourne</t>
-  </si>
-  <si>
     <t>variation_name</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
   </si>
   <si>
     <t>Product No</t>
-  </si>
-  <si>
-    <t>New Drink</t>
   </si>
   <si>
     <t>New Drink 2</t>
@@ -103,6 +94,24 @@
     <t>is_variable
 (is variable for variations
 You can add variations data in Variation Sheet)</t>
+  </si>
+  <si>
+    <t>hello description 1</t>
+  </si>
+  <si>
+    <t>Spiritss</t>
+  </si>
+  <si>
+    <t>hello description 2</t>
+  </si>
+  <si>
+    <t>hello description 3</t>
+  </si>
+  <si>
+    <t>hello description 4</t>
+  </si>
+  <si>
+    <t>hello description 5</t>
   </si>
 </sst>
 </file>
@@ -444,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,7 +469,7 @@
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.140625" customWidth="1"/>
@@ -468,15 +477,15 @@
     <col min="17" max="17" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="165">
+    <row r="1" spans="1:12" ht="90">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -497,13 +506,13 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -511,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D2">
         <v>120</v>
@@ -532,10 +541,10 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -549,36 +558,150 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>110</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
       </c>
       <c r="G3">
         <v>1997</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>110</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>1997</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>1997</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>1997</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
     </row>
@@ -592,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -605,13 +728,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -619,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -630,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -641,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>15</v>

</xml_diff>